<commit_message>
Added full rent feature
</commit_message>
<xml_diff>
--- a/ClientRevenueReportList.xlsx
+++ b/ClientRevenueReportList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juggl\OneDrive\Desktop\Bianca_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4551762A-9F32-4F21-A7DC-5500E074F29C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B13CF3D-558C-4825-A372-9A9C8E0A7466}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1776" yWindow="372" windowWidth="16404" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
   <si>
     <t>Professional</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Suivi - Accompagnement spirituel et énergétique :: Follow-up session - Spiritual and Energetic Guidance</t>
+  </si>
+  <si>
+    <t>Dawson</t>
   </si>
 </sst>
 </file>
@@ -435,11 +438,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1208,6 +1211,26 @@
         <v>90</v>
       </c>
     </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="1">
+        <v>100</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <v>100</v>
+      </c>
+      <c r="H30" s="1">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>